<commit_message>
optimize runtime and update interval list
</commit_message>
<xml_diff>
--- a/data/interval_list.xlsx
+++ b/data/interval_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vanaj\Documents\GitHub\py-encoder-src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76DA3B48-9E07-48DD-B77B-21020B75804B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A9702AE-8FA4-43DC-A08E-DC9824283135}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2520" yWindow="3525" windowWidth="15300" windowHeight="7785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="116">
   <si>
     <t>valid_interval</t>
   </si>
@@ -356,6 +356,18 @@
   </si>
   <si>
     <t>10years</t>
+  </si>
+  <si>
+    <t>5YEARS</t>
+  </si>
+  <si>
+    <t>5 YEARS</t>
+  </si>
+  <si>
+    <t>2400 Hours</t>
+  </si>
+  <si>
+    <t>2years</t>
   </si>
 </sst>
 </file>
@@ -384,7 +396,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -404,6 +416,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -442,7 +460,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -460,6 +478,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -767,10 +788,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B109"/>
+  <dimension ref="A1:B113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
-      <selection activeCell="H105" sqref="H105"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="E111" sqref="E111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1643,10 +1664,42 @@
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A109" s="2" t="s">
+      <c r="A109" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B109" s="6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B110" s="6" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B111" s="7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B112" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B109" s="2" t="s">
+      <c r="B113" s="2" t="s">
         <v>110</v>
       </c>
     </row>

</xml_diff>